<commit_message>
Updated Yaml Setting and Log parsing for performance
</commit_message>
<xml_diff>
--- a/TestData/Results/vnodetest_diag/Test_vnodetest_diag-Cassandra Status Logs 2016-08-24-19-01-36 To 2016-08-24-00-52-40.xlsx
+++ b/TestData/Results/vnodetest_diag/Test_vnodetest_diag-Cassandra Status Logs 2016-08-24-19-01-36 To 2016-08-24-00-52-40.xlsx
@@ -184,13 +184,13 @@
     <t>10.200.178.74</t>
   </si>
   <si>
-    <t>Start Timestamp: 11/21/2016 9:07:59 AM Duration: 00:00:14.3630</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Program: DSEDiagnosticAnalyticParserConsole Version: 3.0.0.15542 Directory: </t>
-  </si>
-  <si>
-    <t>Working Directory: E:\Libraries\Projects\DataStax\Git\DSEDiagnosticAnalyticParser\Binaries</t>
+    <t>Start Timestamp: 11/25/2016 9:34:05 PM Duration: 00:00:17.4910</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Program: DSEDiagnosticAnalyticParserConsole Version: 3.0.0.36443 Directory: </t>
+  </si>
+  <si>
+    <t>Working Directory: E:\Libraries\Projects\DataStax\Git\DSEDiagnosticAnalyticParser\DSEDiagnosticAnalyticParserConsole\bin\x64\Release</t>
   </si>
   <si>
     <t xml:space="preserve">Values: 
@@ -200,13 +200,10 @@
 	--[C]ompactionFlagThresholdInMS 10000 
 	--CompactionFlagThresholdAsIORate|-R 3
 	--SlowLog[Q]ueryThresholdInMS 2000 
-	--SummarizeOnlyOverlappingLogs|-U True
 	--LogStartDate|-Z "1/1/0001 12:00:00 AM" 
 	--LogExcelWorkbook[F]ilter "" 
-	--LoadLogsInto[E]xcel True 
-	--Parse[L]ogs True 
-	--Parse[N]onLogs True 
-	--Parse[A]rchivedLogs True 
+	--Parsing[E]xcelOptions {ParseLoadWorksheets} 
+	--[L]ogParsingExcelOption {ParseLogs} 
 	--Excel[T]emplateFilePath ".\dseTemplate.xlsm" 
 	--ExcelFile[P]ath "C:\Users\Richard\Desktop\Test_vnodetest_diag.xlsm" 
 	--DiagnosticNoSubFolders|-O False 

</xml_diff>